<commit_message>
Added revision for damselfly hybrid species
</commit_message>
<xml_diff>
--- a/Windows/Busquedas/Hybrid/Odonata/Odonata_Hybrids.xlsx
+++ b/Windows/Busquedas/Hybrid/Odonata/Odonata_Hybrids.xlsx
@@ -127,9 +127,6 @@
     <t xml:space="preserve">Lestes sponsa </t>
   </si>
   <si>
-    <t xml:space="preserve">Lestes viridis </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ischnura erratica </t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t xml:space="preserve">Sympecma fusca </t>
   </si>
   <si>
-    <t xml:space="preserve">Ischnura elegans ebneri </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sympatric </t>
   </si>
   <si>
@@ -215,6 +209,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Ischnura elegans</t>
+  </si>
+  <si>
+    <t>Chalcolestes viridis</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,24 +597,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -623,27 +623,27 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -652,27 +652,27 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -681,27 +681,27 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -710,27 +710,27 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -739,27 +739,27 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -768,27 +768,27 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -797,27 +797,27 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -826,27 +826,27 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -855,27 +855,27 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -884,27 +884,27 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -913,27 +913,27 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -942,27 +942,27 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -971,56 +971,56 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1029,27 +1029,27 @@
         <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1058,27 +1058,27 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1087,27 +1087,27 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1116,27 +1116,27 @@
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1145,27 +1145,27 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -1174,27 +1174,27 @@
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -1203,27 +1203,27 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -1232,27 +1232,27 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
@@ -1261,27 +1261,27 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -1290,27 +1290,27 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
@@ -1319,27 +1319,27 @@
         <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -1348,27 +1348,27 @@
         <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -1377,27 +1377,27 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -1406,27 +1406,27 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -1435,27 +1435,27 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1464,27 +1464,27 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -1493,27 +1493,27 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1522,27 +1522,27 @@
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1551,135 +1551,135 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
         <v>33</v>
       </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>